<commit_message>
Update on password rules
</commit_message>
<xml_diff>
--- a/Case Study 1/CSSECDV - Case Study 1 Project Documentation.xlsx
+++ b/Case Study 1/CSSECDV - Case Study 1 Project Documentation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\ejose\Documents\Github\CSSECDV\Case Study 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C6099D0-6D0B-4DC8-B82D-3010F7592B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{032F8DEB-170A-40E4-9886-EA8383F22078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{E5B6E951-E296-6A45-B171-4DEF88B6BA8E}"/>
   </bookViews>
@@ -230,7 +230,7 @@
 3. Symbols (Username): _-.
 4. Symbols (Password): ~`!@#$%^&amp;*()_-+={[}]|\:&lt;,&gt;.?/
 Once the inputs are pre-sanitized, the following must be also met in order to proceed further on the registration process:
-1. Minimum password length of 6
+1. Minimum password length of 8
 2. At least 1 uppercase letter, 1 lowercase letter, 1 number, 1 symbol
 2. Password and confirm password contents match
 3. Username is available
@@ -254,19 +254,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Cascadia Code"/>
+      <family val="3"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Cascadia Code"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -357,51 +355,11 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="11"/>
+        <sz val="12"/>
         <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <name val="Cascadia Code"/>
+        <family val="3"/>
+        <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -422,11 +380,11 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="11"/>
+        <sz val="12"/>
         <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <name val="Cascadia Code"/>
+        <family val="3"/>
+        <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -447,11 +405,11 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="11"/>
+        <sz val="12"/>
         <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <name val="Cascadia Code"/>
+        <family val="3"/>
+        <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -472,11 +430,11 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="11"/>
+        <sz val="12"/>
         <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <name val="Cascadia Code"/>
+        <family val="3"/>
+        <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -501,11 +459,11 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="11"/>
+        <sz val="12"/>
         <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <name val="Cascadia Code"/>
+        <family val="3"/>
+        <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -543,11 +501,51 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Cascadia Code"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Cascadia Code"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -563,14 +561,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BDC2C145-CA6C-4116-8497-301F69D6F2EA}" name="Table1" displayName="Table1" ref="A2:E12" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BDC2C145-CA6C-4116-8497-301F69D6F2EA}" name="Table1" displayName="Table1" ref="A2:E12" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" totalsRowBorderDxfId="5">
   <autoFilter ref="A2:E12" xr:uid="{BDC2C145-CA6C-4116-8497-301F69D6F2EA}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{A8658888-9ED3-4E86-9710-4C5A3B1D4BB8}" name="No." dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{EF8290C0-79ED-4DAC-8965-A7C41CBFEE69}" name="Security Issue" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{DCA9FE58-A714-4D9C-B4D4-FF52664C3540}" name="Java File" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{D7E5722B-2AC8-4CE1-A9D7-5F2C469FBF5C}" name="Possible Vulnerabilities" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{A498D2AB-82DF-4DA5-BF7B-66DE30875766}" name="Solution Implementation" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{A8658888-9ED3-4E86-9710-4C5A3B1D4BB8}" name="No." dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{EF8290C0-79ED-4DAC-8965-A7C41CBFEE69}" name="Security Issue" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{DCA9FE58-A714-4D9C-B4D4-FF52664C3540}" name="Java File" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{D7E5722B-2AC8-4CE1-A9D7-5F2C469FBF5C}" name="Possible Vulnerabilities" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{A498D2AB-82DF-4DA5-BF7B-66DE30875766}" name="Solution Implementation" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -879,23 +877,23 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomRight" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.25" style="1" customWidth="1"/>
+    <col min="2" max="2" width="29.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="42.5" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="90.125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>40</v>
       </c>
@@ -906,7 +904,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -923,7 +921,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="86.25" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -940,7 +938,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="207" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -957,7 +955,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="120.75" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -974,7 +972,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="86.25" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -991,7 +989,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="172.5" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>5</v>
       </c>
@@ -1008,7 +1006,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="207" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -1025,7 +1023,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="210" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="347.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>7</v>
       </c>
@@ -1042,7 +1040,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="224.25" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -1059,7 +1057,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="330" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="396.75" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>9</v>
       </c>
@@ -1076,7 +1074,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="138" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>10</v>
       </c>
@@ -1093,70 +1091,70 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -1164,8 +1162,8 @@
       <c r="E22" s="7"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="64" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="67" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>